<commit_message>
del P+ due to issue
</commit_message>
<xml_diff>
--- a/build/keywords.xlsx
+++ b/build/keywords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Develop\Pulsar\language-sofistik\build\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CA5FBB-4B53-4CC9-9797-87AA84279E72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8849AE-2382-4957-9208-521B96C2FFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21270" firstSheet="18" activeTab="33" xr2:uid="{F1DC097C-994B-40A0-AE10-01AA50F843D6}"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21270" firstSheet="2" activeTab="2" xr2:uid="{F1DC097C-994B-40A0-AE10-01AA50F843D6}"/>
   </bookViews>
   <sheets>
     <sheet name="AQB" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7234" uniqueCount="2610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7234" uniqueCount="2609">
   <si>
     <t>GRP</t>
   </si>
@@ -7885,9 +7885,6 @@
   </si>
   <si>
     <t>GFRB</t>
-  </si>
-  <si>
-    <t>P+</t>
   </si>
 </sst>
 </file>
@@ -23183,8 +23180,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73EFB9C5-8420-44DD-84A3-54AD5FB79C97}">
   <dimension ref="A1:AX54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H53" sqref="H53"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24249,7 +24246,7 @@
         <v>2203</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>2609</v>
+        <v>29</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>2250</v>
@@ -27820,7 +27817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928FE8A4-6029-46B4-A0BD-FBD8644AEC99}">
   <dimension ref="A1:AT45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X20" sqref="X20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add & fix p+
</commit_message>
<xml_diff>
--- a/build/keywords.xlsx
+++ b/build/keywords.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\Develop\Pulsar\language-sofistik\build\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B8849AE-2382-4957-9208-521B96C2FFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EB5DB6C-69A1-4EAD-8591-370B97B1A433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21270" firstSheet="2" activeTab="2" xr2:uid="{F1DC097C-994B-40A0-AE10-01AA50F843D6}"/>
   </bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7234" uniqueCount="2609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7234" uniqueCount="2610">
   <si>
     <t>GRP</t>
   </si>
@@ -7885,6 +7885,9 @@
   </si>
   <si>
     <t>GFRB</t>
+  </si>
+  <si>
+    <t>P+</t>
   </si>
 </sst>
 </file>
@@ -23181,7 +23184,7 @@
   <dimension ref="A1:AX54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -24246,7 +24249,7 @@
         <v>2203</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>29</v>
+        <v>2609</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>2250</v>

</xml_diff>